<commit_message>
modify: 对 excelutil 做下修改,
</commit_message>
<xml_diff>
--- a/src/main/resources/static/excel/内检测数据.xlsx
+++ b/src/main/resources/static/excel/内检测数据.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9084"/>
+    <workbookView windowWidth="23040" windowHeight="9227"/>
   </bookViews>
   <sheets>
     <sheet name="内检测数据" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="17">
   <si>
     <t>里程 m</t>
   </si>
@@ -52,13 +52,13 @@
     <t>INT</t>
   </si>
   <si>
-    <t>AXGR</t>
-  </si>
-  <si>
     <t>EXT</t>
   </si>
   <si>
     <t>CISL</t>
+  </si>
+  <si>
+    <t>AXGR</t>
   </si>
   <si>
     <t>PITT</t>
@@ -72,12 +72,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="h:mm;@"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -111,8 +111,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -125,21 +157,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="等线"/>
@@ -147,8 +164,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,48 +226,10 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -217,48 +242,23 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -277,19 +277,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,37 +301,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,7 +313,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -355,7 +337,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,25 +361,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,43 +433,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,13 +457,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,31 +487,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,30 +536,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -575,159 +545,189 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -743,13 +743,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1076,7 +1076,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -1137,8 +1137,8 @@
       <c r="G2" s="4">
         <v>12</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>11</v>
+      <c r="H2" s="4">
+        <v>111</v>
       </c>
       <c r="I2" s="4">
         <v>0.69</v>
@@ -1146,32 +1146,16 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="E3" s="6">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4">
-        <v>58</v>
-      </c>
-      <c r="G3" s="4">
-        <v>26</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="4">
-        <v>0.7</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4">
@@ -1195,8 +1179,8 @@
       <c r="G4" s="4">
         <v>5</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
+      <c r="H4" s="4">
+        <v>0</v>
       </c>
       <c r="I4" s="4">
         <v>0.69</v>
@@ -1254,7 +1238,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="4">
         <v>0.69</v>
@@ -1326,7 +1310,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5">
         <v>0.239583333333333</v>
@@ -1341,7 +1325,7 @@
         <v>12</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="4">
         <v>0.69</v>
@@ -1355,7 +1339,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D10" s="5">
         <v>0.239583333333333</v>
@@ -1428,7 +1412,7 @@
         <v>9</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" s="4">
         <v>0.69</v>
@@ -1442,7 +1426,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D13" s="5">
         <v>0.5</v>
@@ -1471,7 +1455,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D14" s="5">
         <v>0.239583333333333</v>
@@ -1500,7 +1484,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D15" s="5">
         <v>0.239583333333333</v>
@@ -1515,7 +1499,7 @@
         <v>20</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" s="4">
         <v>0.69</v>
@@ -1558,7 +1542,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="5">
         <v>0.239583333333333</v>
@@ -1602,7 +1586,7 @@
         <v>4</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" s="4">
         <v>0.69</v>
@@ -1703,7 +1687,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D22" s="5">
         <v>0.447916666666667</v>
@@ -1718,7 +1702,7 @@
         <v>9</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I22" s="4">
         <v>0.69</v>
@@ -1732,7 +1716,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D23" s="5">
         <v>0.5</v>
@@ -1776,7 +1760,7 @@
         <v>12</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I24" s="4">
         <v>0.69</v>
@@ -1848,7 +1832,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="5">
         <v>0.239583333333333</v>
@@ -1935,7 +1919,7 @@
         <v>9</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D30" s="5">
         <v>0.239583333333333</v>
@@ -2022,7 +2006,7 @@
         <v>9</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D33" s="5">
         <v>0.5</v>
@@ -2051,7 +2035,7 @@
         <v>9</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D34" s="5">
         <v>0.239583333333333</v>
@@ -2066,7 +2050,7 @@
         <v>12</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I34" s="4">
         <v>0.69</v>
@@ -2138,7 +2122,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D37" s="5">
         <v>0.239583333333333</v>
@@ -2298,7 +2282,7 @@
         <v>8</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I42" s="4">
         <v>0.69</v>
@@ -2312,7 +2296,7 @@
         <v>9</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D43" s="5">
         <v>0.5</v>
@@ -2414,7 +2398,7 @@
         <v>12</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I46" s="4">
         <v>0.69</v>
@@ -2428,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D47" s="5">
         <v>0.239583333333333</v>
@@ -2515,7 +2499,7 @@
         <v>9</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D50" s="5">
         <v>0.239583333333333</v>
@@ -2530,7 +2514,7 @@
         <v>10</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I50" s="4">
         <v>0.69</v>
@@ -2602,7 +2586,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D53" s="5">
         <v>0.5</v>
@@ -2704,7 +2688,7 @@
         <v>16</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I56" s="4">
         <v>0.69</v>
@@ -2718,7 +2702,7 @@
         <v>9</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" s="5">
         <v>0.239583333333333</v>
@@ -2762,7 +2746,7 @@
         <v>4</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I58" s="4">
         <v>0.69</v>
@@ -2805,7 +2789,7 @@
         <v>9</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D60" s="5">
         <v>0.239583333333333</v>
@@ -2878,7 +2862,7 @@
         <v>9</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I62" s="4">
         <v>0.69</v>
@@ -2892,7 +2876,7 @@
         <v>9</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D63" s="5">
         <v>0.5</v>
@@ -2936,7 +2920,7 @@
         <v>12</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I64" s="4">
         <v>0.69</v>
@@ -3008,7 +2992,7 @@
         <v>9</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D67" s="5">
         <v>0.239583333333333</v>
@@ -3023,7 +3007,7 @@
         <v>7</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I67" s="4">
         <v>0.69</v>
@@ -3081,7 +3065,7 @@
         <v>12</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I69" s="4">
         <v>0.69</v>
@@ -3168,7 +3152,7 @@
         <v>8</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I72" s="4">
         <v>0.69</v>
@@ -3182,7 +3166,7 @@
         <v>9</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D73" s="5">
         <v>0.5</v>
@@ -3284,7 +3268,7 @@
         <v>12</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I76" s="4">
         <v>0.69</v>
@@ -3298,7 +3282,7 @@
         <v>9</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D77" s="5">
         <v>0.239583333333333</v>
@@ -3385,7 +3369,7 @@
         <v>9</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D80" s="5">
         <v>0.239583333333333</v>
@@ -3458,7 +3442,7 @@
         <v>9</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I82" s="4">
         <v>0.69</v>
@@ -3472,7 +3456,7 @@
         <v>9</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D83" s="5">
         <v>0.5</v>
@@ -3545,7 +3529,7 @@
         <v>20</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I85" s="4">
         <v>0.69</v>
@@ -3588,7 +3572,7 @@
         <v>9</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D87" s="5">
         <v>0.239583333333333</v>
@@ -3603,7 +3587,7 @@
         <v>7</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I87" s="4">
         <v>0.69</v>
@@ -3661,7 +3645,7 @@
         <v>12</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I89" s="4">
         <v>0.69</v>
@@ -3719,7 +3703,7 @@
         <v>12</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I91" s="4">
         <v>0.69</v>
@@ -3762,7 +3746,7 @@
         <v>9</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D93" s="5">
         <v>0.5</v>
@@ -3777,7 +3761,7 @@
         <v>10</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I93" s="4">
         <v>0.7</v>
@@ -3835,7 +3819,7 @@
         <v>20</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I95" s="4">
         <v>0.69</v>
@@ -3864,7 +3848,7 @@
         <v>16</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I96" s="4">
         <v>0.69</v>
@@ -3878,7 +3862,7 @@
         <v>9</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D97" s="5">
         <v>0.239583333333333</v>
@@ -3893,7 +3877,7 @@
         <v>7</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I97" s="4">
         <v>0.69</v>
@@ -3922,7 +3906,7 @@
         <v>10</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I98" s="4">
         <v>0.69</v>
@@ -3965,7 +3949,7 @@
         <v>9</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D100" s="5">
         <v>0.239583333333333</v>
@@ -4052,7 +4036,7 @@
         <v>9</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D103" s="5">
         <v>0.5</v>
@@ -4067,7 +4051,7 @@
         <v>6</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I103" s="4">
         <v>0.7</v>
@@ -4125,7 +4109,7 @@
         <v>6</v>
       </c>
       <c r="H105" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I105" s="4">
         <v>0.69</v>
@@ -4154,7 +4138,7 @@
         <v>12</v>
       </c>
       <c r="H106" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I106" s="4">
         <v>0.69</v>
@@ -4168,7 +4152,7 @@
         <v>9</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D107" s="5">
         <v>0.239583333333333</v>
@@ -4183,7 +4167,7 @@
         <v>8</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I107" s="4">
         <v>0.69</v>
@@ -4328,7 +4312,7 @@
         <v>27</v>
       </c>
       <c r="H112" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I112" s="4">
         <v>0.69</v>
@@ -4342,7 +4326,7 @@
         <v>9</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D113" s="5">
         <v>0.5</v>
@@ -4357,7 +4341,7 @@
         <v>4</v>
       </c>
       <c r="H113" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I113" s="4">
         <v>0.7</v>
@@ -4386,7 +4370,7 @@
         <v>12</v>
       </c>
       <c r="H114" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I114" s="4">
         <v>0.69</v>
@@ -4415,7 +4399,7 @@
         <v>26</v>
       </c>
       <c r="H115" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I115" s="4">
         <v>0.69</v>
@@ -4444,7 +4428,7 @@
         <v>5</v>
       </c>
       <c r="H116" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I116" s="4">
         <v>0.69</v>
@@ -4458,7 +4442,7 @@
         <v>9</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D117" s="5">
         <v>0.239583333333333</v>
@@ -4473,7 +4457,7 @@
         <v>12</v>
       </c>
       <c r="H117" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I117" s="4">
         <v>0.69</v>
@@ -4545,7 +4529,7 @@
         <v>9</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D120" s="5">
         <v>0.239583333333333</v>
@@ -4632,7 +4616,7 @@
         <v>9</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D123" s="5">
         <v>0.5</v>
@@ -4647,7 +4631,7 @@
         <v>12</v>
       </c>
       <c r="H123" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I123" s="4">
         <v>0.7</v>
@@ -4705,7 +4689,7 @@
         <v>23</v>
       </c>
       <c r="H125" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I125" s="4">
         <v>0.69</v>
@@ -4748,7 +4732,7 @@
         <v>9</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D127" s="5">
         <v>0.239583333333333</v>
@@ -4763,7 +4747,7 @@
         <v>20</v>
       </c>
       <c r="H127" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I127" s="4">
         <v>0.69</v>
@@ -4792,7 +4776,7 @@
         <v>16</v>
       </c>
       <c r="H128" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I128" s="4">
         <v>0.69</v>
@@ -4835,7 +4819,7 @@
         <v>9</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D130" s="5">
         <v>0.239583333333333</v>
@@ -4850,7 +4834,7 @@
         <v>4</v>
       </c>
       <c r="H130" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I130" s="4">
         <v>0.69</v>
@@ -4879,7 +4863,7 @@
         <v>12</v>
       </c>
       <c r="H131" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I131" s="4">
         <v>0.69</v>
@@ -4922,7 +4906,7 @@
         <v>9</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D133" s="5">
         <v>0.5</v>
@@ -4937,7 +4921,7 @@
         <v>12</v>
       </c>
       <c r="H133" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I133" s="4">
         <v>0.7</v>
@@ -5038,7 +5022,7 @@
         <v>9</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D137" s="5">
         <v>0.239583333333333</v>
@@ -5212,7 +5196,7 @@
         <v>9</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D143" s="5">
         <v>0.5</v>
@@ -5328,7 +5312,7 @@
         <v>9</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D147" s="5">
         <v>0.239583333333333</v>
@@ -5343,7 +5327,7 @@
         <v>12</v>
       </c>
       <c r="H147" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I147" s="4">
         <v>0.69</v>
@@ -5401,7 +5385,7 @@
         <v>27</v>
       </c>
       <c r="H149" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I149" s="4">
         <v>0.69</v>
@@ -5415,7 +5399,7 @@
         <v>9</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D150" s="5">
         <v>0.239583333333333</v>
@@ -5459,7 +5443,7 @@
         <v>12</v>
       </c>
       <c r="H151" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I151" s="4">
         <v>0.69</v>
@@ -5502,7 +5486,7 @@
         <v>9</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D153" s="5">
         <v>0.5</v>
@@ -5618,7 +5602,7 @@
         <v>9</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D157" s="5">
         <v>0.239583333333333</v>
@@ -5691,7 +5675,7 @@
         <v>12</v>
       </c>
       <c r="H159" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I159" s="4">
         <v>0.69</v>
@@ -5720,7 +5704,7 @@
         <v>20</v>
       </c>
       <c r="H160" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I160" s="4">
         <v>0.69</v>
@@ -5792,7 +5776,7 @@
         <v>9</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D163" s="5">
         <v>0.5</v>
@@ -5807,7 +5791,7 @@
         <v>6</v>
       </c>
       <c r="H163" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I163" s="4">
         <v>0.7</v>
@@ -5908,7 +5892,7 @@
         <v>9</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D167" s="5">
         <v>0.239583333333333</v>
@@ -5952,7 +5936,7 @@
         <v>27</v>
       </c>
       <c r="H168" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I168" s="4">
         <v>0.69</v>
@@ -5981,7 +5965,7 @@
         <v>12</v>
       </c>
       <c r="H169" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I169" s="4">
         <v>0.69</v>
@@ -6082,7 +6066,7 @@
         <v>9</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D173" s="5">
         <v>0.5</v>
@@ -6198,7 +6182,7 @@
         <v>9</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D177" s="5">
         <v>0.239583333333333</v>
@@ -6227,7 +6211,7 @@
         <v>9</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D178" s="5">
         <v>0.239583333333333</v>
@@ -6242,7 +6226,7 @@
         <v>8</v>
       </c>
       <c r="H178" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I178" s="4">
         <v>0.69</v>
@@ -6329,7 +6313,7 @@
         <v>12</v>
       </c>
       <c r="H181" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I181" s="4">
         <v>0.69</v>
@@ -6372,7 +6356,7 @@
         <v>9</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D183" s="5">
         <v>0.5</v>
@@ -6488,7 +6472,7 @@
         <v>9</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D187" s="5">
         <v>0.239583333333333</v>
@@ -6662,7 +6646,7 @@
         <v>9</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D193" s="5">
         <v>0.5</v>
@@ -6764,7 +6748,7 @@
         <v>12</v>
       </c>
       <c r="H196" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I196" s="4">
         <v>0.69</v>
@@ -6778,7 +6762,7 @@
         <v>9</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D197" s="5">
         <v>0.239583333333333</v>
@@ -6822,7 +6806,7 @@
         <v>27</v>
       </c>
       <c r="H198" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I198" s="4">
         <v>0.69</v>
@@ -6851,7 +6835,7 @@
         <v>12</v>
       </c>
       <c r="H199" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I199" s="4">
         <v>0.69</v>
@@ -6865,7 +6849,7 @@
         <v>9</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D200" s="5">
         <v>0.239583333333333</v>
@@ -6952,7 +6936,7 @@
         <v>9</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D203" s="5">
         <v>0.5</v>
@@ -7068,7 +7052,7 @@
         <v>9</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D207" s="5">
         <v>0.239583333333333</v>
@@ -7141,7 +7125,7 @@
         <v>12</v>
       </c>
       <c r="H209" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I209" s="4">
         <v>0.69</v>
@@ -7228,7 +7212,7 @@
         <v>27</v>
       </c>
       <c r="H212" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I212" s="4">
         <v>0.69</v>
@@ -7242,7 +7226,7 @@
         <v>9</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D213" s="5">
         <v>0.5</v>
@@ -7358,7 +7342,7 @@
         <v>9</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D217" s="5">
         <v>0.239583333333333</v>
@@ -7402,7 +7386,7 @@
         <v>8</v>
       </c>
       <c r="H218" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I218" s="4">
         <v>0.69</v>
@@ -7445,7 +7429,7 @@
         <v>9</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D220" s="5">
         <v>0.239583333333333</v>
@@ -7460,7 +7444,7 @@
         <v>4</v>
       </c>
       <c r="H220" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I220" s="4">
         <v>0.69</v>
@@ -7489,7 +7473,7 @@
         <v>12</v>
       </c>
       <c r="H221" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I221" s="4">
         <v>0.69</v>
@@ -7532,7 +7516,7 @@
         <v>9</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D223" s="5">
         <v>0.5</v>
@@ -7648,7 +7632,7 @@
         <v>9</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D227" s="5">
         <v>0.239583333333333</v>
@@ -7663,7 +7647,7 @@
         <v>20</v>
       </c>
       <c r="H227" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I227" s="4">
         <v>0.69</v>
@@ -7721,7 +7705,7 @@
         <v>12</v>
       </c>
       <c r="H229" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I229" s="4">
         <v>0.69</v>
@@ -7750,7 +7734,7 @@
         <v>12</v>
       </c>
       <c r="H230" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I230" s="4">
         <v>0.69</v>
@@ -7822,7 +7806,7 @@
         <v>9</v>
       </c>
       <c r="C233" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D233" s="5">
         <v>0.5</v>
@@ -7938,7 +7922,7 @@
         <v>9</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D237" s="5">
         <v>0.239583333333333</v>
@@ -8025,7 +8009,7 @@
         <v>9</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D240" s="5">
         <v>0.239583333333333</v>
@@ -8069,7 +8053,7 @@
         <v>12</v>
       </c>
       <c r="H241" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I241" s="4">
         <v>0.69</v>
@@ -8112,7 +8096,7 @@
         <v>9</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D243" s="5">
         <v>0.5</v>
@@ -8228,7 +8212,7 @@
         <v>9</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D247" s="5">
         <v>0.239583333333333</v>
@@ -8388,7 +8372,7 @@
         <v>27</v>
       </c>
       <c r="H252" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I252" s="4">
         <v>0.69</v>
@@ -8402,7 +8386,7 @@
         <v>9</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D253" s="5">
         <v>0.5</v>
@@ -8417,7 +8401,7 @@
         <v>4</v>
       </c>
       <c r="H253" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I253" s="4">
         <v>0.7</v>
@@ -8518,7 +8502,7 @@
         <v>9</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D257" s="5">
         <v>0.239583333333333</v>
@@ -8605,7 +8589,7 @@
         <v>9</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D260" s="5">
         <v>0.239583333333333</v>
@@ -8692,7 +8676,7 @@
         <v>9</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D263" s="5">
         <v>0.5</v>
@@ -8808,7 +8792,7 @@
         <v>9</v>
       </c>
       <c r="C267" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D267" s="5">
         <v>0.239583333333333</v>
@@ -8823,7 +8807,7 @@
         <v>12</v>
       </c>
       <c r="H267" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I267" s="4">
         <v>0.69</v>
@@ -8852,7 +8836,7 @@
         <v>8</v>
       </c>
       <c r="H268" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I268" s="4">
         <v>0.69</v>
@@ -8881,7 +8865,7 @@
         <v>27</v>
       </c>
       <c r="H269" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I269" s="4">
         <v>0.69</v>
@@ -8895,7 +8879,7 @@
         <v>9</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D270" s="5">
         <v>0.239583333333333</v>
@@ -8982,7 +8966,7 @@
         <v>9</v>
       </c>
       <c r="C273" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D273" s="5">
         <v>0.5</v>
@@ -9098,7 +9082,7 @@
         <v>9</v>
       </c>
       <c r="C277" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D277" s="5">
         <v>0.239583333333333</v>
@@ -9113,7 +9097,7 @@
         <v>20</v>
       </c>
       <c r="H277" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I277" s="4">
         <v>0.69</v>
@@ -9200,7 +9184,7 @@
         <v>12</v>
       </c>
       <c r="H280" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I280" s="4">
         <v>0.69</v>
@@ -9272,7 +9256,7 @@
         <v>9</v>
       </c>
       <c r="C283" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D283" s="5">
         <v>0.5</v>
@@ -9345,7 +9329,7 @@
         <v>26</v>
       </c>
       <c r="H285" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I285" s="4">
         <v>0.69</v>
@@ -9388,7 +9372,7 @@
         <v>9</v>
       </c>
       <c r="C287" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D287" s="5">
         <v>0.239583333333333</v>
@@ -9475,7 +9459,7 @@
         <v>9</v>
       </c>
       <c r="C290" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D290" s="5">
         <v>0.239583333333333</v>
@@ -9707,7 +9691,7 @@
         <v>9</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D298" s="5">
         <v>0.239583333333333</v>
@@ -9722,7 +9706,7 @@
         <v>4</v>
       </c>
       <c r="H298" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I298" s="4">
         <v>0.69</v>
@@ -9751,7 +9735,7 @@
         <v>12</v>
       </c>
       <c r="H299" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I299" s="4">
         <v>0.69</v>
@@ -9780,7 +9764,7 @@
         <v>26</v>
       </c>
       <c r="H300" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I300" s="4">
         <v>0.69</v>
@@ -9823,7 +9807,7 @@
         <v>9</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D302" s="5">
         <v>0.239583333333333</v>
@@ -9997,7 +9981,7 @@
         <v>9</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D308" s="5">
         <v>0.239583333333333</v>
@@ -10070,7 +10054,7 @@
         <v>12</v>
       </c>
       <c r="H310" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I310" s="4">
         <v>0.69</v>
@@ -10099,7 +10083,7 @@
         <v>22</v>
       </c>
       <c r="H311" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I311" s="4">
         <v>0.7</v>
@@ -10113,7 +10097,7 @@
         <v>9</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D312" s="5">
         <v>0.239583333333333</v>
@@ -10287,7 +10271,7 @@
         <v>9</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D318" s="5">
         <v>0.239583333333333</v>
@@ -10331,7 +10315,7 @@
         <v>14</v>
       </c>
       <c r="H319" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I319" s="4">
         <v>0.69</v>
@@ -10389,7 +10373,7 @@
         <v>22</v>
       </c>
       <c r="H321" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I321" s="4">
         <v>0.7</v>
@@ -10403,7 +10387,7 @@
         <v>9</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D322" s="5">
         <v>0.239583333333333</v>
@@ -10461,7 +10445,7 @@
         <v>9</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D324" s="5">
         <v>0.239583333333333</v>
@@ -10505,7 +10489,7 @@
         <v>16</v>
       </c>
       <c r="H325" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I325" s="4">
         <v>0.69</v>
@@ -10563,7 +10547,7 @@
         <v>4</v>
       </c>
       <c r="H327" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I327" s="4">
         <v>0.69</v>
@@ -10621,7 +10605,7 @@
         <v>10</v>
       </c>
       <c r="H329" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I329" s="4">
         <v>0.69</v>
@@ -10635,7 +10619,7 @@
         <v>9</v>
       </c>
       <c r="C330" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D330" s="5">
         <v>0.5</v>
@@ -10751,7 +10735,7 @@
         <v>9</v>
       </c>
       <c r="C334" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D334" s="5">
         <v>0.239583333333333</v>
@@ -10766,7 +10750,7 @@
         <v>20</v>
       </c>
       <c r="H334" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I334" s="4">
         <v>0.69</v>
@@ -10838,7 +10822,7 @@
         <v>9</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D337" s="5">
         <v>0.239583333333333</v>
@@ -10882,7 +10866,7 @@
         <v>12</v>
       </c>
       <c r="H338" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I338" s="4">
         <v>0.69</v>
@@ -10911,7 +10895,7 @@
         <v>27</v>
       </c>
       <c r="H339" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I339" s="4">
         <v>0.69</v>
@@ -10925,7 +10909,7 @@
         <v>9</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D340" s="5">
         <v>0.5</v>
@@ -10940,7 +10924,7 @@
         <v>4</v>
       </c>
       <c r="H340" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I340" s="4">
         <v>0.7</v>
@@ -10998,7 +10982,7 @@
         <v>26</v>
       </c>
       <c r="H342" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I342" s="4">
         <v>0.69</v>
@@ -11027,7 +11011,7 @@
         <v>5</v>
       </c>
       <c r="H343" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I343" s="4">
         <v>0.69</v>
@@ -11041,7 +11025,7 @@
         <v>9</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D344" s="5">
         <v>0.239583333333333</v>
@@ -11172,7 +11156,7 @@
         <v>12</v>
       </c>
       <c r="H348" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I348" s="4">
         <v>0.69</v>
@@ -11186,7 +11170,7 @@
         <v>9</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D349" s="5">
         <v>0.239583333333333</v>
@@ -11273,7 +11257,7 @@
         <v>9</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D352" s="5">
         <v>0.5</v>
@@ -11375,7 +11359,7 @@
         <v>5</v>
       </c>
       <c r="H355" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I355" s="4">
         <v>0.69</v>
@@ -11389,7 +11373,7 @@
         <v>9</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D356" s="5">
         <v>0.239583333333333</v>
@@ -11433,7 +11417,7 @@
         <v>8</v>
       </c>
       <c r="H357" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I357" s="4">
         <v>0.69</v>
@@ -11476,7 +11460,7 @@
         <v>9</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D359" s="5">
         <v>0.239583333333333</v>
@@ -11491,7 +11475,7 @@
         <v>4</v>
       </c>
       <c r="H359" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I359" s="4">
         <v>0.69</v>
@@ -11563,7 +11547,7 @@
         <v>9</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D362" s="5">
         <v>0.5</v>
@@ -11665,7 +11649,7 @@
         <v>12</v>
       </c>
       <c r="H365" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I365" s="4">
         <v>0.69</v>
@@ -11679,7 +11663,7 @@
         <v>9</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D366" s="5">
         <v>0.239583333333333</v>
@@ -11723,7 +11707,7 @@
         <v>27</v>
       </c>
       <c r="H367" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I367" s="4">
         <v>0.69</v>
@@ -11752,7 +11736,7 @@
         <v>12</v>
       </c>
       <c r="H368" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I368" s="4">
         <v>0.69</v>
@@ -11839,7 +11823,7 @@
         <v>27</v>
       </c>
       <c r="H371" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I371" s="4">
         <v>0.69</v>
@@ -11853,7 +11837,7 @@
         <v>9</v>
       </c>
       <c r="C372" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D372" s="5">
         <v>0.5</v>
@@ -11969,7 +11953,7 @@
         <v>9</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D376" s="5">
         <v>0.239583333333333</v>
@@ -11984,7 +11968,7 @@
         <v>12</v>
       </c>
       <c r="H376" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I376" s="4">
         <v>0.69</v>
@@ -12056,7 +12040,7 @@
         <v>9</v>
       </c>
       <c r="C379" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D379" s="5">
         <v>0.239583333333333</v>
@@ -12071,7 +12055,7 @@
         <v>12</v>
       </c>
       <c r="H379" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I379" s="4">
         <v>0.69</v>
@@ -12245,7 +12229,7 @@
         <v>5</v>
       </c>
       <c r="H385" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I385" s="7">
         <v>0.69</v>
@@ -12288,7 +12272,7 @@
         <v>9</v>
       </c>
       <c r="C387" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D387" s="5">
         <v>0.239583333333333</v>
@@ -12303,7 +12287,7 @@
         <v>4</v>
       </c>
       <c r="H387" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I387" s="7">
         <v>0.69</v>
@@ -12404,7 +12388,7 @@
         <v>9</v>
       </c>
       <c r="C391" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D391" s="5">
         <v>0.239583333333333</v>
@@ -12448,7 +12432,7 @@
         <v>12</v>
       </c>
       <c r="H392" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I392" s="7">
         <v>0.69</v>
@@ -12506,7 +12490,7 @@
         <v>5</v>
       </c>
       <c r="H394" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I394" s="7">
         <v>0.69</v>
@@ -12578,7 +12562,7 @@
         <v>9</v>
       </c>
       <c r="C397" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D397" s="5">
         <v>0.239583333333333</v>
@@ -12593,7 +12577,7 @@
         <v>10</v>
       </c>
       <c r="H397" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I397" s="7">
         <v>0.69</v>
@@ -12680,7 +12664,7 @@
         <v>22</v>
       </c>
       <c r="H400" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I400" s="7">
         <v>0.7</v>
@@ -12694,7 +12678,7 @@
         <v>9</v>
       </c>
       <c r="C401" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D401" s="5">
         <v>0.239583333333333</v>
@@ -12767,7 +12751,7 @@
         <v>14</v>
       </c>
       <c r="H403" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I403" s="7">
         <v>0.69</v>
@@ -12854,7 +12838,7 @@
         <v>22</v>
       </c>
       <c r="H406" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I406" s="7">
         <v>0.69</v>
@@ -12868,7 +12852,7 @@
         <v>9</v>
       </c>
       <c r="C407" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D407" s="5">
         <v>0.239583333333333</v>
@@ -12970,7 +12954,7 @@
         <v>22</v>
       </c>
       <c r="H410" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I410" s="7">
         <v>0.7</v>
@@ -12984,7 +12968,7 @@
         <v>9</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D411" s="5">
         <v>0.239583333333333</v>

</xml_diff>